<commit_message>
add links to excel
</commit_message>
<xml_diff>
--- a/DevBoardList.xlsx
+++ b/DevBoardList.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Dokumente_HDD\## TO SORT\Basteln\Projekte\DevBoardList\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7C86462-B0F0-498B-B809-E2EC22C20663}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51DD303D-1A92-4DDD-84E0-E2C5A65C3C44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="162" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="162" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -118,7 +118,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="107">
   <si>
     <t>ATmega32U4</t>
   </si>
@@ -459,6 +459,18 @@
   </si>
   <si>
     <t>BOARD</t>
+  </si>
+  <si>
+    <t>https://www.seeedstudio.com/XIAO-RP2040-v1-0-p-5026.html</t>
+  </si>
+  <si>
+    <t>https://de.aliexpress.com/item/1005003928558306.html</t>
+  </si>
+  <si>
+    <t>https://www.tomshardware.com/best-picks/best-rp2040-boards</t>
+  </si>
+  <si>
+    <t>https://golem.hu/guide/controllers/</t>
   </si>
 </sst>
 </file>
@@ -566,7 +578,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="41">
+  <borders count="50">
     <border>
       <left/>
       <right/>
@@ -1094,13 +1106,124 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="1" tint="0.14999847407452621"/>
+      </left>
+      <right style="thin">
+        <color theme="1" tint="0.14999847407452621"/>
+      </right>
+      <top style="thin">
+        <color theme="1" tint="0.14999847407452621"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="1" tint="0.14999847407452621"/>
+      </left>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color theme="1" tint="0.14999847407452621"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="1" tint="0.14999847407452621"/>
+      </left>
+      <right style="medium">
+        <color theme="1" tint="0.14996795556505021"/>
+      </right>
+      <top style="thin">
+        <color theme="1" tint="0.14999847407452621"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="1" tint="0.14999847407452621"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="1" tint="0.14999847407452621"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="1" tint="0.14999847407452621"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color theme="1" tint="0.14996795556505021"/>
+      </left>
+      <right style="thin">
+        <color theme="1" tint="0.14999847407452621"/>
+      </right>
+      <top style="thin">
+        <color theme="1" tint="0.14999847407452621"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="1" tint="0.14993743705557422"/>
+      </left>
+      <right style="thin">
+        <color theme="1" tint="0.14993743705557422"/>
+      </right>
+      <top style="thin">
+        <color theme="1" tint="0.14999847407452621"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="1" tint="0.14993743705557422"/>
+      </left>
+      <right style="thin">
+        <color theme="1" tint="0.14999847407452621"/>
+      </right>
+      <top style="thin">
+        <color theme="1" tint="0.14999847407452621"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color theme="1" tint="0.14999847407452621"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="113">
+  <cellXfs count="143">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -1241,7 +1364,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1265,8 +1388,8 @@
     <xf numFmtId="0" fontId="7" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1288,12 +1411,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1334,11 +1453,9 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1398,7 +1515,6 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1410,6 +1526,111 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="41" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="41" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="42" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="41" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="41" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="41" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="43" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="44" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="44" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="42" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="41" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="45" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="41" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="47" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="46" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="41" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1419,24 +1640,6 @@
     <cellStyle name="Währung" xfId="1" builtinId="4"/>
   </cellStyles>
   <dxfs count="46">
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color theme="1" tint="0.14999847407452621"/>
-        </left>
-        <right style="thick">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color theme="1" tint="0.14999847407452621"/>
-        </top>
-        <bottom style="thin">
-          <color theme="1" tint="0.14999847407452621"/>
-        </bottom>
-        <vertical/>
-      </border>
-    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1471,13 +1674,14 @@
       </font>
     </dxf>
     <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <numFmt numFmtId="20" formatCode="dd/\ mmm\ yy"/>
+      <alignment textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color theme="1" tint="0.14999847407452621"/>
         </left>
-        <right style="thick">
-          <color indexed="64"/>
+        <right style="thin">
+          <color theme="1" tint="0.14999847407452621"/>
         </right>
         <top style="thin">
           <color theme="1" tint="0.14999847407452621"/>
@@ -1485,8 +1689,31 @@
         <bottom style="thin">
           <color theme="1" tint="0.14999847407452621"/>
         </bottom>
+        <vertical style="thin">
+          <color theme="1" tint="0.14999847407452621"/>
+        </vertical>
+        <horizontal style="thin">
+          <color theme="1" tint="0.14999847407452621"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="20" formatCode="dd/\ mmm\ yy"/>
+      <alignment textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color theme="1" tint="0.14996795556505021"/>
+        </left>
+        <right style="thin">
+          <color theme="1" tint="0.14999847407452621"/>
+        </right>
+        <top style="thin">
+          <color theme="1" tint="0.14999847407452621"/>
+        </top>
+        <bottom style="thin">
+          <color theme="1" tint="0.14999847407452621"/>
+        </bottom>
         <vertical/>
-        <horizontal/>
       </border>
     </dxf>
     <dxf>
@@ -1506,148 +1733,6 @@
         </bottom>
         <vertical/>
         <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color theme="1" tint="0.14999847407452621"/>
-        </left>
-        <right style="thick">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color theme="1" tint="0.14999847407452621"/>
-        </top>
-        <bottom style="thin">
-          <color theme="1" tint="0.14999847407452621"/>
-        </bottom>
-        <vertical/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color theme="1" tint="0.14999847407452621"/>
-        </left>
-        <right style="thick">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color theme="1" tint="0.14999847407452621"/>
-        </top>
-        <bottom style="thin">
-          <color theme="1" tint="0.14999847407452621"/>
-        </bottom>
-        <vertical/>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0&quot; Pin&quot;"/>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color theme="1" tint="0.14999847407452621"/>
-        </left>
-        <right style="thick">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color theme="1" tint="0.14999847407452621"/>
-        </top>
-        <bottom style="thin">
-          <color theme="1" tint="0.14999847407452621"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="20" formatCode="dd/\ mmm\ yy"/>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color theme="1" tint="0.14999847407452621"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color theme="1" tint="0.14999847407452621"/>
-        </top>
-        <bottom style="thin">
-          <color theme="1" tint="0.14999847407452621"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color theme="1" tint="0.14999847407452621"/>
-        </top>
-        <bottom style="thin">
-          <color theme="1" tint="0.14999847407452621"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="20" formatCode="dd/\ mmm\ yy"/>
-      <alignment textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color theme="1" tint="0.14999847407452621"/>
-        </left>
-        <right style="thin">
-          <color theme="1" tint="0.14999847407452621"/>
-        </right>
-        <top style="thin">
-          <color theme="1" tint="0.14999847407452621"/>
-        </top>
-        <bottom style="thin">
-          <color theme="1" tint="0.14999847407452621"/>
-        </bottom>
-        <vertical style="thin">
-          <color theme="1" tint="0.14999847407452621"/>
-        </vertical>
-        <horizontal style="thin">
-          <color theme="1" tint="0.14999847407452621"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="20" formatCode="dd/\ mmm\ yy"/>
-      <alignment textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="medium">
-          <color theme="1" tint="0.14996795556505021"/>
-        </left>
-        <right style="thin">
-          <color theme="1" tint="0.14999847407452621"/>
-        </right>
-        <top style="thin">
-          <color theme="1" tint="0.14999847407452621"/>
-        </top>
-        <bottom style="thin">
-          <color theme="1" tint="0.14999847407452621"/>
-        </bottom>
-        <vertical/>
       </border>
     </dxf>
     <dxf>
@@ -1771,6 +1856,24 @@
       </border>
     </dxf>
     <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color theme="1" tint="0.14999847407452621"/>
+        </left>
+        <right style="thick">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color theme="1" tint="0.14999847407452621"/>
+        </top>
+        <bottom style="thin">
+          <color theme="1" tint="0.14999847407452621"/>
+        </bottom>
+        <vertical/>
+      </border>
+    </dxf>
+    <dxf>
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
@@ -1886,6 +1989,24 @@
         <left style="thin">
           <color theme="1" tint="0.14999847407452621"/>
         </left>
+        <right style="thick">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color theme="1" tint="0.14999847407452621"/>
+        </top>
+        <bottom style="thin">
+          <color theme="1" tint="0.14999847407452621"/>
+        </bottom>
+        <vertical/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color theme="1" tint="0.14999847407452621"/>
+        </left>
         <right style="thin">
           <color theme="1" tint="0.14999847407452621"/>
         </right>
@@ -1942,6 +2063,25 @@
       </border>
     </dxf>
     <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color theme="1" tint="0.14999847407452621"/>
+        </left>
+        <right style="thick">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color theme="1" tint="0.14999847407452621"/>
+        </top>
+        <bottom style="thin">
+          <color theme="1" tint="0.14999847407452621"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="166" formatCode="0&quot;V&quot;"/>
       <alignment horizontal="left" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
@@ -2013,6 +2153,23 @@
       <border diagonalUp="0" diagonalDown="0">
         <left/>
         <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color theme="1" tint="0.14999847407452621"/>
+        </top>
+        <bottom style="thin">
+          <color theme="1" tint="0.14999847407452621"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
           <color theme="1" tint="0.14999847407452621"/>
         </right>
         <top style="thin">
@@ -2052,6 +2209,44 @@
         <left style="thin">
           <color theme="1" tint="0.14999847407452621"/>
         </left>
+        <right style="thick">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color theme="1" tint="0.14999847407452621"/>
+        </top>
+        <bottom style="thin">
+          <color theme="1" tint="0.14999847407452621"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0&quot; Pin&quot;"/>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color theme="1" tint="0.14999847407452621"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color theme="1" tint="0.14999847407452621"/>
+        </top>
+        <bottom style="thin">
+          <color theme="1" tint="0.14999847407452621"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="20" formatCode="dd/\ mmm\ yy"/>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color theme="1" tint="0.14999847407452621"/>
+        </left>
         <right/>
         <top style="thin">
           <color theme="1" tint="0.14999847407452621"/>
@@ -2134,6 +2329,24 @@
         </bottom>
         <vertical/>
         <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color theme="1" tint="0.14999847407452621"/>
+        </left>
+        <right style="thick">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color theme="1" tint="0.14999847407452621"/>
+        </top>
+        <bottom style="thin">
+          <color theme="1" tint="0.14999847407452621"/>
+        </bottom>
+        <vertical/>
       </border>
     </dxf>
     <dxf>
@@ -2213,6 +2426,14 @@
         <bottom style="thick">
           <color theme="1" tint="0.14996795556505021"/>
         </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <bottom/>
       </border>
     </dxf>
   </dxfs>
@@ -3237,50 +3458,50 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E0176607-7D05-4F53-9667-39A4A03C5F12}" name="Tabelle1" displayName="Tabelle1" ref="A2:AM17" totalsRowShown="0" headerRowDxfId="13" headerRowBorderDxfId="45">
-  <autoFilter ref="A2:AM17" xr:uid="{E0176607-7D05-4F53-9667-39A4A03C5F12}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E0176607-7D05-4F53-9667-39A4A03C5F12}" name="Tabelle1" displayName="Tabelle1" ref="A2:AM19" totalsRowShown="0" headerRowDxfId="45" headerRowBorderDxfId="44">
+  <autoFilter ref="A2:AM19" xr:uid="{E0176607-7D05-4F53-9667-39A4A03C5F12}"/>
   <tableColumns count="39">
-    <tableColumn id="10" xr3:uid="{06F3FDFB-D908-4506-9F73-B1950B5432B2}" name="id &lt;inv&gt;" dataDxfId="44"/>
-    <tableColumn id="1" xr3:uid="{50E4B843-3F3C-48AB-9A11-A8AEAE98C688}" name="name" dataDxfId="43"/>
-    <tableColumn id="2" xr3:uid="{BDC1F6FD-F5BE-4BDC-A530-120CF1EDB073}" name="image &lt;value of id&gt;" dataDxfId="42">
+    <tableColumn id="10" xr3:uid="{06F3FDFB-D908-4506-9F73-B1950B5432B2}" name="id &lt;inv&gt;" dataDxfId="43"/>
+    <tableColumn id="1" xr3:uid="{50E4B843-3F3C-48AB-9A11-A8AEAE98C688}" name="name" dataDxfId="42"/>
+    <tableColumn id="2" xr3:uid="{BDC1F6FD-F5BE-4BDC-A530-120CF1EDB073}" name="image &lt;value of id&gt;" dataDxfId="41">
       <calculatedColumnFormula>_xlfn.IMAGE("https://m.media-amazon.com/images/I/71A63A5j3bL._AC_UF894,1000_QL80_.jpg")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{7FA666B0-D25B-4777-954C-48E52AB85516}" name="imageSrc &lt;inv&gt;" dataDxfId="0" dataCellStyle="Link"/>
-    <tableColumn id="13" xr3:uid="{E026474B-EDC8-4862-82FC-4A495BD8B4BE}" name="link" dataDxfId="41" dataCellStyle="Link"/>
-    <tableColumn id="27" xr3:uid="{B4944D22-4754-4CF0-83EE-1AC37F1784DC}" name="price" dataDxfId="40" dataCellStyle="Währung"/>
-    <tableColumn id="19" xr3:uid="{64BA4BF5-1FDE-4732-B0F4-123756491263}" name="dimX" dataDxfId="39"/>
-    <tableColumn id="21" xr3:uid="{E38615C3-81C4-47AD-8AC2-915CF0103F19}" name="dimY" dataDxfId="38"/>
-    <tableColumn id="7" xr3:uid="{65EE9DA7-A351-431B-AAE5-4B1E8D342B2C}" name="connector" dataDxfId="11"/>
-    <tableColumn id="22" xr3:uid="{55C0C826-652F-4A6B-83E3-CCDB9601F342}" name="docs _x000a_&lt;value of id&gt;" dataDxfId="37"/>
-    <tableColumn id="28" xr3:uid="{CAF68D57-9DD5-418C-9725-8DDA560DAC4E}" name="docsSrc &lt;inv&gt;" dataDxfId="10"/>
-    <tableColumn id="3" xr3:uid="{587542E2-02C3-42C4-B632-57BFD8B68620}" name="chip" dataDxfId="36" dataCellStyle="Währung"/>
-    <tableColumn id="31" xr3:uid="{E487950B-DA55-4A5A-AA67-C3DE24DF1FC2}" name="cDocs _x000a_&lt;value of controller&gt;" dataDxfId="35"/>
-    <tableColumn id="33" xr3:uid="{0B976E26-FBA6-46F9-A18C-6EF982C84981}" name="cDocsSrc &lt;inv&gt;" dataDxfId="12"/>
-    <tableColumn id="4" xr3:uid="{63C6D974-BDD1-4CA5-BB22-CAB3EEB46821}" name="clock" dataDxfId="34"/>
-    <tableColumn id="30" xr3:uid="{36D840AA-FA68-4B34-86C5-8F75852AECBE}" name="coreCnt" dataDxfId="33"/>
-    <tableColumn id="34" xr3:uid="{63D7B924-8924-40BF-A9EB-4E62ADBF30B1}" name="coreBit" dataDxfId="32"/>
-    <tableColumn id="8" xr3:uid="{74F9564F-F54A-4208-BF89-F5B2185537B4}" name="voltOp" dataDxfId="31"/>
-    <tableColumn id="24" xr3:uid="{D241F3B3-FAE1-413D-881F-5705D2DF3FA7}" name="voltIn" dataDxfId="6"/>
-    <tableColumn id="5" xr3:uid="{8B0B2852-1E23-43D9-8CCF-612E7B5EAC8E}" name="sizeFlash" dataDxfId="30"/>
-    <tableColumn id="35" xr3:uid="{250AF3D6-1439-4360-AC53-5AFE236521E6}" name="sizeFlashFree" dataDxfId="29"/>
-    <tableColumn id="15" xr3:uid="{CE6EB7FE-073F-47E9-8438-3EA045DA63E9}" name="sizeRAM" dataDxfId="28"/>
-    <tableColumn id="16" xr3:uid="{71571936-9667-47A6-8DEC-607A17E73107}" name="sizeEPROM" dataDxfId="9"/>
-    <tableColumn id="20" xr3:uid="{7FB941BC-C54B-4F39-9306-34F9620C7AEC}" name="pinout &lt;value of id&gt;" dataDxfId="27"/>
-    <tableColumn id="38" xr3:uid="{18A4EFC4-8BA0-438D-A1F7-FFF1849C3013}" name="pinoutSrc &lt;inv&gt;" dataDxfId="26"/>
-    <tableColumn id="23" xr3:uid="{AC87607F-8794-435F-BC6D-EDBFEA907F02}" name="cntGPIO" dataDxfId="25"/>
-    <tableColumn id="6" xr3:uid="{ECC27E07-5954-4DED-8238-0ED81C119069}" name="cntDigital" dataDxfId="24"/>
-    <tableColumn id="18" xr3:uid="{B8D9FA3A-1ED0-4F23-A9F0-AC177FD12812}" name="cntAnalog" dataDxfId="23"/>
-    <tableColumn id="39" xr3:uid="{5B23A253-6588-47DA-BC8E-D2C1D9B7D92B}" name="analogBit" dataDxfId="22"/>
-    <tableColumn id="17" xr3:uid="{CD2A34BE-45F2-4510-8EF9-83EDDFEE035A}" name="cntPWM" dataDxfId="8"/>
-    <tableColumn id="29" xr3:uid="{10C0EFDD-8FEE-41FA-A6DA-8FE3EA458520}" name="laneUART" dataDxfId="21"/>
-    <tableColumn id="37" xr3:uid="{8718023C-E89D-479D-8DDB-53B56190C652}" name="langeI2C" dataDxfId="20"/>
-    <tableColumn id="36" xr3:uid="{0A52E200-5A7E-4345-B763-2510161760F2}" name="laneSPI" dataDxfId="19"/>
-    <tableColumn id="25" xr3:uid="{1C1B65FF-0397-4A72-B697-BEE8A7130ACE}" name="WLAN &lt;protocol&gt;" dataDxfId="18"/>
-    <tableColumn id="26" xr3:uid="{CE794EDB-081C-414E-8975-5B0FBFC905EE}" name="BT &lt;protocol&gt;" dataDxfId="17"/>
-    <tableColumn id="14" xr3:uid="{D2D192E4-D4BC-456C-AFD4-2AC6C192B221}" name="HID &lt;protocol&gt;" dataDxfId="16"/>
+    <tableColumn id="11" xr3:uid="{7FA666B0-D25B-4777-954C-48E52AB85516}" name="imageSrc &lt;inv&gt;" dataDxfId="40" dataCellStyle="Link"/>
+    <tableColumn id="13" xr3:uid="{E026474B-EDC8-4862-82FC-4A495BD8B4BE}" name="link" dataDxfId="39" dataCellStyle="Link"/>
+    <tableColumn id="27" xr3:uid="{B4944D22-4754-4CF0-83EE-1AC37F1784DC}" name="price" dataDxfId="38" dataCellStyle="Währung"/>
+    <tableColumn id="19" xr3:uid="{64BA4BF5-1FDE-4732-B0F4-123756491263}" name="dimX" dataDxfId="37"/>
+    <tableColumn id="21" xr3:uid="{E38615C3-81C4-47AD-8AC2-915CF0103F19}" name="dimY" dataDxfId="36"/>
+    <tableColumn id="7" xr3:uid="{65EE9DA7-A351-431B-AAE5-4B1E8D342B2C}" name="connector" dataDxfId="35"/>
+    <tableColumn id="22" xr3:uid="{55C0C826-652F-4A6B-83E3-CCDB9601F342}" name="docs _x000a_&lt;value of id&gt;" dataDxfId="34"/>
+    <tableColumn id="28" xr3:uid="{CAF68D57-9DD5-418C-9725-8DDA560DAC4E}" name="docsSrc &lt;inv&gt;" dataDxfId="33"/>
+    <tableColumn id="3" xr3:uid="{587542E2-02C3-42C4-B632-57BFD8B68620}" name="chip" dataDxfId="32" dataCellStyle="Währung"/>
+    <tableColumn id="31" xr3:uid="{E487950B-DA55-4A5A-AA67-C3DE24DF1FC2}" name="cDocs _x000a_&lt;value of controller&gt;" dataDxfId="31"/>
+    <tableColumn id="33" xr3:uid="{0B976E26-FBA6-46F9-A18C-6EF982C84981}" name="cDocsSrc &lt;inv&gt;" dataDxfId="30"/>
+    <tableColumn id="4" xr3:uid="{63C6D974-BDD1-4CA5-BB22-CAB3EEB46821}" name="clock" dataDxfId="29"/>
+    <tableColumn id="30" xr3:uid="{36D840AA-FA68-4B34-86C5-8F75852AECBE}" name="coreCnt" dataDxfId="28"/>
+    <tableColumn id="34" xr3:uid="{63D7B924-8924-40BF-A9EB-4E62ADBF30B1}" name="coreBit" dataDxfId="27"/>
+    <tableColumn id="8" xr3:uid="{74F9564F-F54A-4208-BF89-F5B2185537B4}" name="voltOp" dataDxfId="26"/>
+    <tableColumn id="24" xr3:uid="{D241F3B3-FAE1-413D-881F-5705D2DF3FA7}" name="voltIn" dataDxfId="25"/>
+    <tableColumn id="5" xr3:uid="{8B0B2852-1E23-43D9-8CCF-612E7B5EAC8E}" name="sizeFlash" dataDxfId="24"/>
+    <tableColumn id="35" xr3:uid="{250AF3D6-1439-4360-AC53-5AFE236521E6}" name="sizeFlashFree" dataDxfId="23"/>
+    <tableColumn id="15" xr3:uid="{CE6EB7FE-073F-47E9-8438-3EA045DA63E9}" name="sizeRAM" dataDxfId="22"/>
+    <tableColumn id="16" xr3:uid="{71571936-9667-47A6-8DEC-607A17E73107}" name="sizeEPROM" dataDxfId="21"/>
+    <tableColumn id="20" xr3:uid="{7FB941BC-C54B-4F39-9306-34F9620C7AEC}" name="pinout &lt;value of id&gt;" dataDxfId="20"/>
+    <tableColumn id="38" xr3:uid="{18A4EFC4-8BA0-438D-A1F7-FFF1849C3013}" name="pinoutSrc &lt;inv&gt;" dataDxfId="19"/>
+    <tableColumn id="23" xr3:uid="{AC87607F-8794-435F-BC6D-EDBFEA907F02}" name="cntGPIO" dataDxfId="18"/>
+    <tableColumn id="6" xr3:uid="{ECC27E07-5954-4DED-8238-0ED81C119069}" name="cntDigital" dataDxfId="17"/>
+    <tableColumn id="18" xr3:uid="{B8D9FA3A-1ED0-4F23-A9F0-AC177FD12812}" name="cntAnalog" dataDxfId="16"/>
+    <tableColumn id="39" xr3:uid="{5B23A253-6588-47DA-BC8E-D2C1D9B7D92B}" name="analogBit" dataDxfId="15"/>
+    <tableColumn id="17" xr3:uid="{CD2A34BE-45F2-4510-8EF9-83EDDFEE035A}" name="cntPWM" dataDxfId="14"/>
+    <tableColumn id="29" xr3:uid="{10C0EFDD-8FEE-41FA-A6DA-8FE3EA458520}" name="laneUART" dataDxfId="13"/>
+    <tableColumn id="37" xr3:uid="{8718023C-E89D-479D-8DDB-53B56190C652}" name="langeI2C" dataDxfId="12"/>
+    <tableColumn id="36" xr3:uid="{0A52E200-5A7E-4345-B763-2510161760F2}" name="laneSPI" dataDxfId="11"/>
+    <tableColumn id="25" xr3:uid="{1C1B65FF-0397-4A72-B697-BEE8A7130ACE}" name="WLAN &lt;protocol&gt;" dataDxfId="10"/>
+    <tableColumn id="26" xr3:uid="{CE794EDB-081C-414E-8975-5B0FBFC905EE}" name="BT &lt;protocol&gt;" dataDxfId="9"/>
+    <tableColumn id="14" xr3:uid="{D2D192E4-D4BC-456C-AFD4-2AC6C192B221}" name="HID &lt;protocol&gt;" dataDxfId="8"/>
     <tableColumn id="32" xr3:uid="{2BDB4DB9-DFE3-4AAA-95E1-062F62CF4291}" name="castellatedEdge" dataDxfId="7"/>
-    <tableColumn id="12" xr3:uid="{9E7D0881-B1D1-43E9-B469-F3EA9BF57CBF}" name="platform" dataDxfId="15"/>
-    <tableColumn id="9" xr3:uid="{72928A24-D14D-468F-8CE2-67C7ED1B739C}" name="comment" dataDxfId="14"/>
+    <tableColumn id="12" xr3:uid="{9E7D0881-B1D1-43E9-B469-F3EA9BF57CBF}" name="platform" dataDxfId="6"/>
+    <tableColumn id="9" xr3:uid="{72928A24-D14D-468F-8CE2-67C7ED1B739C}" name="comment" dataDxfId="5"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3549,100 +3770,93 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AM17"/>
+  <dimension ref="A1:AM19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="W1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AD4" sqref="AD4"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.7109375" style="65" customWidth="1"/>
-    <col min="2" max="2" width="21" style="65" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="27" style="65" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.7109375" style="66" customWidth="1"/>
-    <col min="5" max="5" width="6.5703125" style="65" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.7109375" style="65" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="7.85546875" style="65" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="24.7109375" style="65" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="12" style="65" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="20.85546875" style="65" customWidth="1"/>
-    <col min="13" max="13" width="20.7109375" style="65" customWidth="1"/>
-    <col min="14" max="14" width="8.7109375" style="65" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="8.28515625" style="65" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="8.28515625" style="65" customWidth="1"/>
+    <col min="1" max="1" width="6.7109375" customWidth="1"/>
+    <col min="2" max="2" width="21" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.7109375" style="49" customWidth="1"/>
+    <col min="5" max="5" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="24.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="12" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="20.85546875" customWidth="1"/>
+    <col min="13" max="13" width="20.7109375" customWidth="1"/>
+    <col min="14" max="14" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="8.28515625" customWidth="1"/>
     <col min="17" max="17" width="11.28515625" style="48" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="9.5703125" style="65" customWidth="1"/>
-    <col min="19" max="19" width="10.7109375" style="65" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="11.28515625" style="65" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="11.28515625" style="65" customWidth="1"/>
-    <col min="22" max="22" width="11" style="65" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="10.85546875" style="65" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="9.5703125" customWidth="1"/>
+    <col min="19" max="19" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="11.28515625" customWidth="1"/>
+    <col min="22" max="22" width="11" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="10.85546875" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="21.5703125" style="48" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="17.42578125" style="48" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="7.85546875" style="48" bestFit="1" customWidth="1"/>
     <col min="27" max="27" width="9" style="48" bestFit="1" customWidth="1"/>
     <col min="28" max="28" width="9.42578125" style="48" bestFit="1" customWidth="1"/>
     <col min="29" max="29" width="9.42578125" style="48" customWidth="1"/>
-    <col min="30" max="30" width="8.28515625" style="67" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="8.28515625" style="65" bestFit="1" customWidth="1"/>
     <col min="31" max="31" width="7.7109375" style="48" customWidth="1"/>
     <col min="32" max="32" width="10.85546875" style="48" bestFit="1" customWidth="1"/>
     <col min="33" max="33" width="9.85546875" style="48" bestFit="1" customWidth="1"/>
     <col min="34" max="34" width="11.5703125" style="48" customWidth="1"/>
     <col min="35" max="35" width="11.140625" style="48" customWidth="1"/>
-    <col min="36" max="36" width="11.5703125" style="67" customWidth="1"/>
-    <col min="37" max="37" width="17.28515625" style="67" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="13.28515625" style="65" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="30.7109375" style="65" bestFit="1" customWidth="1"/>
-    <col min="40" max="16384" width="9.140625" style="65"/>
+    <col min="36" max="36" width="11.5703125" style="65" customWidth="1"/>
+    <col min="37" max="37" width="17.28515625" style="65" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="30.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:39" s="83" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="83" t="s">
+    <row r="1" spans="1:39" s="56" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="56" t="s">
         <v>102</v>
       </c>
-      <c r="B1" s="56"/>
-      <c r="C1" s="56"/>
-      <c r="D1" s="68"/>
-      <c r="E1" s="107" t="s">
+      <c r="D1" s="66"/>
+      <c r="E1" s="80" t="s">
         <v>91</v>
       </c>
-      <c r="F1" s="56"/>
-      <c r="G1" s="56"/>
-      <c r="H1" s="56"/>
-      <c r="I1" s="56"/>
       <c r="J1" s="57"/>
-      <c r="K1" s="68"/>
-      <c r="L1" s="82" t="s">
+      <c r="K1" s="66"/>
+      <c r="L1" s="80" t="s">
         <v>97</v>
       </c>
-      <c r="N1" s="82"/>
-      <c r="Q1" s="84"/>
-      <c r="S1" s="85"/>
-      <c r="T1" s="82" t="s">
+      <c r="N1" s="80"/>
+      <c r="Q1" s="81"/>
+      <c r="S1" s="66"/>
+      <c r="T1" s="80" t="s">
         <v>99</v>
       </c>
-      <c r="W1" s="85"/>
-      <c r="X1" s="86" t="s">
+      <c r="W1" s="66"/>
+      <c r="X1" s="82" t="s">
         <v>98</v>
       </c>
-      <c r="Y1" s="84"/>
-      <c r="Z1" s="84"/>
-      <c r="AA1" s="84"/>
-      <c r="AB1" s="84"/>
-      <c r="AC1" s="84"/>
-      <c r="AD1" s="87"/>
-      <c r="AE1" s="86" t="s">
+      <c r="Y1" s="81"/>
+      <c r="Z1" s="81"/>
+      <c r="AA1" s="81"/>
+      <c r="AB1" s="81"/>
+      <c r="AC1" s="81"/>
+      <c r="AD1" s="83"/>
+      <c r="AE1" s="82" t="s">
         <v>100</v>
       </c>
-      <c r="AF1" s="84"/>
-      <c r="AG1" s="84"/>
-      <c r="AH1" s="84"/>
-      <c r="AI1" s="84"/>
-      <c r="AJ1" s="88"/>
-      <c r="AK1" s="87"/>
-      <c r="AL1" s="82" t="s">
+      <c r="AF1" s="81"/>
+      <c r="AG1" s="81"/>
+      <c r="AH1" s="81"/>
+      <c r="AI1" s="81"/>
+      <c r="AJ1" s="84"/>
+      <c r="AK1" s="83"/>
+      <c r="AL1" s="80" t="s">
         <v>101</v>
       </c>
     </row>
@@ -3656,7 +3870,7 @@
       <c r="C2" s="52" t="s">
         <v>87</v>
       </c>
-      <c r="D2" s="69" t="s">
+      <c r="D2" s="67" t="s">
         <v>77</v>
       </c>
       <c r="E2" s="51" t="s">
@@ -3677,7 +3891,7 @@
       <c r="J2" s="52" t="s">
         <v>96</v>
       </c>
-      <c r="K2" s="69" t="s">
+      <c r="K2" s="67" t="s">
         <v>95</v>
       </c>
       <c r="L2" s="51" t="s">
@@ -3701,7 +3915,7 @@
       <c r="R2" s="53" t="s">
         <v>59</v>
       </c>
-      <c r="S2" s="73" t="s">
+      <c r="S2" s="71" t="s">
         <v>74</v>
       </c>
       <c r="T2" s="51" t="s">
@@ -3713,7 +3927,7 @@
       <c r="V2" s="51" t="s">
         <v>62</v>
       </c>
-      <c r="W2" s="73" t="s">
+      <c r="W2" s="71" t="s">
         <v>63</v>
       </c>
       <c r="X2" s="52" t="s">
@@ -3734,7 +3948,7 @@
       <c r="AC2" s="53" t="s">
         <v>83</v>
       </c>
-      <c r="AD2" s="79" t="s">
+      <c r="AD2" s="77" t="s">
         <v>67</v>
       </c>
       <c r="AE2" s="53" t="s">
@@ -3755,7 +3969,7 @@
       <c r="AJ2" s="55" t="s">
         <v>86</v>
       </c>
-      <c r="AK2" s="91" t="s">
+      <c r="AK2" s="87" t="s">
         <v>90</v>
       </c>
       <c r="AL2" s="54" t="s">
@@ -3765,7 +3979,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="3" spans="1:39" customFormat="1" ht="87.95" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:39" ht="87.95" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A3" s="37">
         <v>1</v>
       </c>
@@ -3773,8 +3987,8 @@
         <v>28</v>
       </c>
       <c r="C3" s="5"/>
-      <c r="D3" s="109"/>
-      <c r="E3" s="108"/>
+      <c r="D3" s="104"/>
+      <c r="E3" s="103"/>
       <c r="F3" s="12">
         <v>4</v>
       </c>
@@ -3784,11 +3998,11 @@
       <c r="H3" s="17">
         <v>7</v>
       </c>
-      <c r="I3" s="99" t="s">
+      <c r="I3" s="95" t="s">
         <v>7</v>
       </c>
-      <c r="J3" s="100"/>
-      <c r="K3" s="72"/>
+      <c r="J3" s="96"/>
+      <c r="K3" s="70"/>
       <c r="L3" s="42" t="s">
         <v>0</v>
       </c>
@@ -3806,17 +4020,17 @@
       <c r="R3" s="11">
         <v>5</v>
       </c>
-      <c r="S3" s="74" t="s">
+      <c r="S3" s="72" t="s">
         <v>24</v>
       </c>
-      <c r="T3" s="94" t="s">
+      <c r="T3" s="90" t="s">
         <v>8</v>
       </c>
       <c r="U3" s="44"/>
       <c r="V3" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="W3" s="74" t="s">
+      <c r="W3" s="72" t="s">
         <v>3</v>
       </c>
       <c r="X3" s="45" t="e" vm="1">
@@ -3834,10 +4048,10 @@
         <v>9</v>
       </c>
       <c r="AC3" s="20"/>
-      <c r="AD3" s="80">
+      <c r="AD3" s="78">
         <v>5</v>
       </c>
-      <c r="AE3" s="77">
+      <c r="AE3" s="75">
         <v>1</v>
       </c>
       <c r="AF3" s="30">
@@ -3855,10 +4069,10 @@
       <c r="AJ3" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="AK3" s="92" t="s">
+      <c r="AK3" s="88" t="s">
         <v>5</v>
       </c>
-      <c r="AL3" s="89" t="s">
+      <c r="AL3" s="85" t="s">
         <v>4</v>
       </c>
       <c r="AM3" s="7" t="s">
@@ -3872,7 +4086,7 @@
       <c r="B4" s="33" t="s">
         <v>33</v>
       </c>
-      <c r="D4" s="110"/>
+      <c r="D4" s="105"/>
       <c r="F4" s="13">
         <v>6</v>
       </c>
@@ -3882,11 +4096,11 @@
       <c r="H4" s="24">
         <v>7</v>
       </c>
-      <c r="I4" s="101" t="s">
+      <c r="I4" s="97" t="s">
         <v>6</v>
       </c>
-      <c r="J4" s="102"/>
-      <c r="K4" s="98"/>
+      <c r="J4" s="98"/>
+      <c r="K4" s="94"/>
       <c r="L4" s="40" t="s">
         <v>0</v>
       </c>
@@ -3902,7 +4116,7 @@
       <c r="R4" s="14">
         <v>5</v>
       </c>
-      <c r="S4" s="76" t="s">
+      <c r="S4" s="74" t="s">
         <v>24</v>
       </c>
       <c r="T4" s="44" t="s">
@@ -3912,7 +4126,7 @@
       <c r="V4" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="W4" s="74" t="s">
+      <c r="W4" s="72" t="s">
         <v>3</v>
       </c>
       <c r="X4" s="45" t="e" vm="1">
@@ -3930,10 +4144,10 @@
         <v>9</v>
       </c>
       <c r="AC4" s="20"/>
-      <c r="AD4" s="81">
+      <c r="AD4" s="79">
         <v>5</v>
       </c>
-      <c r="AE4" s="78">
+      <c r="AE4" s="76">
         <v>1</v>
       </c>
       <c r="AF4" s="31">
@@ -3951,10 +4165,10 @@
       <c r="AJ4" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="AK4" s="93" t="s">
+      <c r="AK4" s="89" t="s">
         <v>5</v>
       </c>
-      <c r="AL4" s="89" t="s">
+      <c r="AL4" s="85" t="s">
         <v>4</v>
       </c>
       <c r="AM4" s="7" t="s">
@@ -3968,7 +4182,7 @@
       <c r="B5" s="33" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="110"/>
+      <c r="D5" s="105"/>
       <c r="F5" s="13">
         <v>2</v>
       </c>
@@ -3978,16 +4192,16 @@
       <c r="H5" s="24">
         <v>10</v>
       </c>
-      <c r="I5" s="101" t="s">
+      <c r="I5" s="97" t="s">
         <v>7</v>
       </c>
-      <c r="J5" s="102"/>
-      <c r="K5" s="98"/>
+      <c r="J5" s="98"/>
+      <c r="K5" s="94"/>
       <c r="L5" s="40" t="s">
         <v>20</v>
       </c>
-      <c r="M5" s="95"/>
-      <c r="N5" s="96"/>
+      <c r="M5" s="91"/>
+      <c r="N5" s="92"/>
       <c r="O5" s="59">
         <v>160</v>
       </c>
@@ -3998,7 +4212,7 @@
       <c r="R5" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="S5" s="76" t="s">
+      <c r="S5" s="74" t="s">
         <v>25</v>
       </c>
       <c r="T5" s="41" t="s">
@@ -4008,7 +4222,7 @@
       <c r="V5" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="W5" s="75" t="s">
+      <c r="W5" s="73" t="s">
         <v>26</v>
       </c>
       <c r="X5" s="46" t="e" vm="2">
@@ -4026,10 +4240,10 @@
         <v>18</v>
       </c>
       <c r="AC5" s="21"/>
-      <c r="AD5" s="81">
+      <c r="AD5" s="79">
         <v>9</v>
       </c>
-      <c r="AE5" s="78">
+      <c r="AE5" s="76">
         <v>1</v>
       </c>
       <c r="AF5" s="31">
@@ -4047,10 +4261,10 @@
       <c r="AJ5" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="AK5" s="93" t="s">
+      <c r="AK5" s="89" t="s">
         <v>5</v>
       </c>
-      <c r="AL5" s="89" t="s">
+      <c r="AL5" s="85" t="s">
         <v>4</v>
       </c>
       <c r="AM5" s="3"/>
@@ -4063,7 +4277,7 @@
         <v>14</v>
       </c>
       <c r="C6" s="38"/>
-      <c r="D6" s="110"/>
+      <c r="D6" s="105"/>
       <c r="F6" s="13">
         <v>5</v>
       </c>
@@ -4073,16 +4287,16 @@
       <c r="H6" s="24">
         <v>8</v>
       </c>
-      <c r="I6" s="101" t="s">
+      <c r="I6" s="97" t="s">
         <v>7</v>
       </c>
-      <c r="J6" s="102"/>
-      <c r="K6" s="71"/>
+      <c r="J6" s="98"/>
+      <c r="K6" s="69"/>
       <c r="L6" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="M6" s="97"/>
-      <c r="N6" s="97"/>
+      <c r="M6" s="93"/>
+      <c r="N6" s="93"/>
       <c r="O6" s="59">
         <v>133</v>
       </c>
@@ -4093,7 +4307,7 @@
       <c r="R6" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="S6" s="76" t="s">
+      <c r="S6" s="74" t="s">
         <v>19</v>
       </c>
       <c r="T6" s="41" t="s">
@@ -4103,7 +4317,7 @@
       <c r="V6" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="W6" s="75" t="s">
+      <c r="W6" s="73" t="s">
         <v>26</v>
       </c>
       <c r="X6" s="46" t="e" vm="3">
@@ -4121,10 +4335,10 @@
         <v>40</v>
       </c>
       <c r="AC6" s="21"/>
-      <c r="AD6" s="81">
+      <c r="AD6" s="79">
         <v>16</v>
       </c>
-      <c r="AE6" s="78">
+      <c r="AE6" s="76">
         <v>2</v>
       </c>
       <c r="AF6" s="31">
@@ -4142,10 +4356,10 @@
       <c r="AJ6" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="AK6" s="93" t="s">
+      <c r="AK6" s="89" t="s">
         <v>1</v>
       </c>
-      <c r="AL6" s="89" t="s">
+      <c r="AL6" s="85" t="s">
         <v>27</v>
       </c>
       <c r="AM6" s="3"/>
@@ -4158,7 +4372,7 @@
         <v>34</v>
       </c>
       <c r="C7" s="38"/>
-      <c r="D7" s="110"/>
+      <c r="D7" s="105"/>
       <c r="F7" s="13">
         <v>5</v>
       </c>
@@ -4168,16 +4382,16 @@
       <c r="H7" s="24">
         <v>8</v>
       </c>
-      <c r="I7" s="103" t="s">
+      <c r="I7" s="99" t="s">
         <v>6</v>
       </c>
-      <c r="J7" s="104"/>
-      <c r="K7" s="71"/>
+      <c r="J7" s="100"/>
+      <c r="K7" s="69"/>
       <c r="L7" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="M7" s="97"/>
-      <c r="N7" s="97"/>
+      <c r="M7" s="93"/>
+      <c r="N7" s="93"/>
       <c r="O7" s="59">
         <v>133</v>
       </c>
@@ -4188,7 +4402,7 @@
       <c r="R7" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="S7" s="76" t="s">
+      <c r="S7" s="74" t="s">
         <v>19</v>
       </c>
       <c r="T7" s="41" t="s">
@@ -4198,7 +4412,7 @@
       <c r="V7" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="W7" s="75" t="s">
+      <c r="W7" s="73" t="s">
         <v>26</v>
       </c>
       <c r="X7" s="46" t="e" vm="4">
@@ -4216,10 +4430,10 @@
         <v>40</v>
       </c>
       <c r="AC7" s="21"/>
-      <c r="AD7" s="81">
+      <c r="AD7" s="79">
         <v>16</v>
       </c>
-      <c r="AE7" s="78">
+      <c r="AE7" s="76">
         <v>2</v>
       </c>
       <c r="AF7" s="31">
@@ -4237,10 +4451,10 @@
       <c r="AJ7" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="AK7" s="93" t="s">
+      <c r="AK7" s="89" t="s">
         <v>5</v>
       </c>
-      <c r="AL7" s="89" t="s">
+      <c r="AL7" s="85" t="s">
         <v>27</v>
       </c>
       <c r="AM7" s="3"/>
@@ -4252,7 +4466,7 @@
       <c r="B8" s="33" t="s">
         <v>35</v>
       </c>
-      <c r="D8" s="110"/>
+      <c r="D8" s="105"/>
       <c r="F8" s="13">
         <v>5</v>
       </c>
@@ -4262,11 +4476,11 @@
       <c r="H8" s="24">
         <v>7</v>
       </c>
-      <c r="I8" s="105" t="s">
+      <c r="I8" s="101" t="s">
         <v>6</v>
       </c>
-      <c r="J8" s="106"/>
-      <c r="K8" s="72"/>
+      <c r="J8" s="102"/>
+      <c r="K8" s="70"/>
       <c r="L8" s="43" t="s">
         <v>15</v>
       </c>
@@ -4282,7 +4496,7 @@
       <c r="R8" s="35">
         <v>3.3</v>
       </c>
-      <c r="S8" s="76" t="s">
+      <c r="S8" s="74" t="s">
         <v>19</v>
       </c>
       <c r="T8" s="41" t="s">
@@ -4292,7 +4506,7 @@
       <c r="V8" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="W8" s="75" t="s">
+      <c r="W8" s="73" t="s">
         <v>26</v>
       </c>
       <c r="X8" s="46" t="s">
@@ -4309,10 +4523,10 @@
         <v>41</v>
       </c>
       <c r="AC8" s="21"/>
-      <c r="AD8" s="81">
+      <c r="AD8" s="79">
         <v>16</v>
       </c>
-      <c r="AE8" s="78">
+      <c r="AE8" s="76">
         <v>2</v>
       </c>
       <c r="AF8" s="31">
@@ -4330,10 +4544,10 @@
       <c r="AJ8" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="AK8" s="93" t="s">
+      <c r="AK8" s="89" t="s">
         <v>5</v>
       </c>
-      <c r="AL8" s="89" t="s">
+      <c r="AL8" s="85" t="s">
         <v>27</v>
       </c>
       <c r="AM8" s="3" t="s">
@@ -4348,7 +4562,7 @@
         <v>36</v>
       </c>
       <c r="C9"/>
-      <c r="D9" s="111"/>
+      <c r="D9" s="106"/>
       <c r="E9"/>
       <c r="F9" s="13">
         <v>5</v>
@@ -4359,11 +4573,11 @@
       <c r="H9" s="24">
         <v>7</v>
       </c>
-      <c r="I9" s="105" t="s">
+      <c r="I9" s="101" t="s">
         <v>6</v>
       </c>
-      <c r="J9" s="106"/>
-      <c r="K9" s="72"/>
+      <c r="J9" s="102"/>
+      <c r="K9" s="70"/>
       <c r="L9" s="43" t="s">
         <v>15</v>
       </c>
@@ -4379,7 +4593,7 @@
       <c r="R9" s="35">
         <v>3.3</v>
       </c>
-      <c r="S9" s="76" t="s">
+      <c r="S9" s="74" t="s">
         <v>19</v>
       </c>
       <c r="T9" s="41" t="s">
@@ -4389,7 +4603,7 @@
       <c r="V9" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="W9" s="75" t="s">
+      <c r="W9" s="73" t="s">
         <v>26</v>
       </c>
       <c r="X9" s="46" t="e" vm="5">
@@ -4407,7 +4621,7 @@
         <v>41</v>
       </c>
       <c r="AC9" s="21"/>
-      <c r="AD9" s="81">
+      <c r="AD9" s="79">
         <v>16</v>
       </c>
       <c r="AE9" s="47">
@@ -4428,10 +4642,10 @@
       <c r="AJ9" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="AK9" s="93" t="s">
+      <c r="AK9" s="89" t="s">
         <v>1</v>
       </c>
-      <c r="AL9" s="89" t="s">
+      <c r="AL9" s="85" t="s">
         <v>27</v>
       </c>
       <c r="AM9" s="3"/>
@@ -4444,7 +4658,7 @@
         <v>38</v>
       </c>
       <c r="C10"/>
-      <c r="D10" s="111"/>
+      <c r="D10" s="106"/>
       <c r="E10"/>
       <c r="F10" s="13">
         <v>4</v>
@@ -4455,11 +4669,11 @@
       <c r="H10" s="24">
         <v>7</v>
       </c>
-      <c r="I10" s="105" t="s">
+      <c r="I10" s="101" t="s">
         <v>6</v>
       </c>
-      <c r="J10" s="106"/>
-      <c r="K10" s="72"/>
+      <c r="J10" s="102"/>
+      <c r="K10" s="70"/>
       <c r="L10" s="43" t="s">
         <v>15</v>
       </c>
@@ -4475,7 +4689,7 @@
       <c r="R10" s="35">
         <v>3.3</v>
       </c>
-      <c r="S10" s="76" t="s">
+      <c r="S10" s="74" t="s">
         <v>19</v>
       </c>
       <c r="T10" s="41" t="s">
@@ -4485,7 +4699,7 @@
       <c r="V10" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="W10" s="75" t="s">
+      <c r="W10" s="73" t="s">
         <v>26</v>
       </c>
       <c r="X10" s="46" t="e" vm="6">
@@ -4503,10 +4717,10 @@
         <v>41</v>
       </c>
       <c r="AC10" s="21"/>
-      <c r="AD10" s="81">
+      <c r="AD10" s="79">
         <v>16</v>
       </c>
-      <c r="AE10" s="78">
+      <c r="AE10" s="76">
         <v>2</v>
       </c>
       <c r="AF10" s="31">
@@ -4524,10 +4738,10 @@
       <c r="AJ10" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="AK10" s="93" t="s">
+      <c r="AK10" s="89" t="s">
         <v>1</v>
       </c>
-      <c r="AL10" s="89" t="s">
+      <c r="AL10" s="85" t="s">
         <v>27</v>
       </c>
       <c r="AM10" s="3"/>
@@ -4540,7 +4754,7 @@
         <v>46</v>
       </c>
       <c r="C11"/>
-      <c r="D11" s="111"/>
+      <c r="D11" s="106"/>
       <c r="E11"/>
       <c r="F11" s="13">
         <v>3</v>
@@ -4551,11 +4765,11 @@
       <c r="H11" s="24">
         <v>7</v>
       </c>
-      <c r="I11" s="105" t="s">
+      <c r="I11" s="101" t="s">
         <v>6</v>
       </c>
-      <c r="J11" s="106"/>
-      <c r="K11" s="72"/>
+      <c r="J11" s="102"/>
+      <c r="K11" s="70"/>
       <c r="L11" s="43" t="s">
         <v>15</v>
       </c>
@@ -4571,7 +4785,7 @@
       <c r="R11" s="35">
         <v>3.3</v>
       </c>
-      <c r="S11" s="76" t="s">
+      <c r="S11" s="74" t="s">
         <v>19</v>
       </c>
       <c r="T11" s="41" t="s">
@@ -4581,7 +4795,7 @@
       <c r="V11" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="W11" s="75" t="s">
+      <c r="W11" s="73" t="s">
         <v>26</v>
       </c>
       <c r="X11" s="46" t="e" vm="7">
@@ -4599,10 +4813,10 @@
         <v>41</v>
       </c>
       <c r="AC11" s="21"/>
-      <c r="AD11" s="81">
+      <c r="AD11" s="79">
         <v>16</v>
       </c>
-      <c r="AE11" s="78">
+      <c r="AE11" s="76">
         <v>2</v>
       </c>
       <c r="AF11" s="31">
@@ -4620,10 +4834,10 @@
       <c r="AJ11" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="AK11" s="93" t="s">
+      <c r="AK11" s="89" t="s">
         <v>1</v>
       </c>
-      <c r="AL11" s="89" t="s">
+      <c r="AL11" s="85" t="s">
         <v>27</v>
       </c>
       <c r="AM11" s="3"/>
@@ -4634,13 +4848,13 @@
       </c>
       <c r="B12" s="34"/>
       <c r="C12" s="39"/>
-      <c r="D12" s="112"/>
+      <c r="D12" s="107"/>
       <c r="E12" s="40"/>
       <c r="G12" s="16"/>
       <c r="H12" s="24"/>
       <c r="I12" s="18"/>
       <c r="J12" s="17"/>
-      <c r="K12" s="70"/>
+      <c r="K12" s="68"/>
       <c r="L12" s="41"/>
       <c r="M12" s="41"/>
       <c r="N12" s="64"/>
@@ -4650,26 +4864,26 @@
       <c r="P12" s="26"/>
       <c r="Q12" s="26"/>
       <c r="R12" s="14"/>
-      <c r="S12" s="76"/>
+      <c r="S12" s="74"/>
       <c r="T12" s="41"/>
       <c r="U12" s="41"/>
       <c r="V12" s="2"/>
-      <c r="W12" s="76"/>
+      <c r="W12" s="74"/>
       <c r="X12" s="47"/>
       <c r="Y12" s="47"/>
       <c r="Z12" s="4"/>
       <c r="AA12" s="4"/>
       <c r="AB12" s="4"/>
       <c r="AC12" s="21"/>
-      <c r="AD12" s="81"/>
-      <c r="AE12" s="78"/>
+      <c r="AD12" s="79"/>
+      <c r="AE12" s="76"/>
       <c r="AF12" s="31"/>
       <c r="AG12" s="29"/>
       <c r="AH12" s="15"/>
       <c r="AI12" s="15"/>
       <c r="AJ12" s="23"/>
-      <c r="AK12" s="93"/>
-      <c r="AL12" s="90"/>
+      <c r="AK12" s="89"/>
+      <c r="AL12" s="86"/>
       <c r="AM12" s="3"/>
     </row>
     <row r="13" spans="1:39" s="1" customFormat="1" ht="87.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -4682,14 +4896,16 @@
       <c r="C13" s="39" t="s">
         <v>23</v>
       </c>
-      <c r="D13" s="112"/>
-      <c r="E13" s="40"/>
+      <c r="D13" s="107"/>
+      <c r="E13" s="40" t="s">
+        <v>103</v>
+      </c>
       <c r="F13" s="13"/>
       <c r="G13" s="16"/>
       <c r="H13" s="24"/>
       <c r="I13" s="19"/>
       <c r="J13" s="24"/>
-      <c r="K13" s="70"/>
+      <c r="K13" s="68"/>
       <c r="L13" s="41"/>
       <c r="M13" s="41"/>
       <c r="N13" s="64"/>
@@ -4697,26 +4913,26 @@
       <c r="P13" s="26"/>
       <c r="Q13" s="26"/>
       <c r="R13" s="14"/>
-      <c r="S13" s="76"/>
+      <c r="S13" s="74"/>
       <c r="T13" s="41"/>
       <c r="U13" s="41"/>
       <c r="V13" s="2"/>
-      <c r="W13" s="76"/>
+      <c r="W13" s="74"/>
       <c r="X13" s="47"/>
       <c r="Y13" s="47"/>
       <c r="Z13" s="4"/>
       <c r="AA13" s="4"/>
       <c r="AB13" s="4"/>
       <c r="AC13" s="21"/>
-      <c r="AD13" s="81"/>
-      <c r="AE13" s="78"/>
+      <c r="AD13" s="79"/>
+      <c r="AE13" s="76"/>
       <c r="AF13" s="31"/>
       <c r="AG13" s="29"/>
       <c r="AH13" s="15"/>
       <c r="AI13" s="15"/>
       <c r="AJ13" s="23"/>
-      <c r="AK13" s="93"/>
-      <c r="AL13" s="90"/>
+      <c r="AK13" s="89"/>
+      <c r="AL13" s="86"/>
       <c r="AM13" s="3"/>
     </row>
     <row r="14" spans="1:39" s="1" customFormat="1" ht="87.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -4729,14 +4945,14 @@
       <c r="C14" s="39" t="s">
         <v>48</v>
       </c>
-      <c r="D14" s="112"/>
+      <c r="D14" s="107"/>
       <c r="E14" s="40"/>
       <c r="F14" s="13"/>
       <c r="G14" s="16"/>
       <c r="H14" s="24"/>
       <c r="I14" s="19"/>
       <c r="J14" s="24"/>
-      <c r="K14" s="70"/>
+      <c r="K14" s="68"/>
       <c r="L14" s="41"/>
       <c r="M14" s="41"/>
       <c r="N14" s="64"/>
@@ -4744,26 +4960,26 @@
       <c r="P14" s="26"/>
       <c r="Q14" s="26"/>
       <c r="R14" s="14"/>
-      <c r="S14" s="76"/>
+      <c r="S14" s="74"/>
       <c r="T14" s="41"/>
       <c r="U14" s="41"/>
       <c r="V14" s="2"/>
-      <c r="W14" s="76"/>
+      <c r="W14" s="74"/>
       <c r="X14" s="47"/>
       <c r="Y14" s="47"/>
       <c r="Z14" s="4"/>
       <c r="AA14" s="4"/>
       <c r="AB14" s="4"/>
       <c r="AC14" s="21"/>
-      <c r="AD14" s="81"/>
-      <c r="AE14" s="78"/>
+      <c r="AD14" s="79"/>
+      <c r="AE14" s="76"/>
       <c r="AF14" s="31"/>
       <c r="AG14" s="29"/>
       <c r="AH14" s="15"/>
       <c r="AI14" s="15"/>
       <c r="AJ14" s="23"/>
-      <c r="AK14" s="93"/>
-      <c r="AL14" s="90"/>
+      <c r="AK14" s="89"/>
+      <c r="AL14" s="86"/>
       <c r="AM14" s="3"/>
     </row>
     <row r="15" spans="1:39" s="1" customFormat="1" ht="87.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -4776,14 +4992,14 @@
       <c r="C15" s="39" t="s">
         <v>50</v>
       </c>
-      <c r="D15" s="112"/>
+      <c r="D15" s="107"/>
       <c r="E15" s="40"/>
       <c r="F15" s="13"/>
       <c r="G15" s="16"/>
       <c r="H15" s="24"/>
       <c r="I15" s="19"/>
       <c r="J15" s="24"/>
-      <c r="K15" s="70"/>
+      <c r="K15" s="68"/>
       <c r="L15" s="41"/>
       <c r="M15" s="41"/>
       <c r="N15" s="64"/>
@@ -4791,26 +5007,26 @@
       <c r="P15" s="26"/>
       <c r="Q15" s="26"/>
       <c r="R15" s="14"/>
-      <c r="S15" s="76"/>
+      <c r="S15" s="74"/>
       <c r="T15" s="41"/>
       <c r="U15" s="41"/>
       <c r="V15" s="2"/>
-      <c r="W15" s="76"/>
+      <c r="W15" s="74"/>
       <c r="X15" s="47"/>
       <c r="Y15" s="47"/>
       <c r="Z15" s="4"/>
       <c r="AA15" s="4"/>
       <c r="AB15" s="4"/>
       <c r="AC15" s="21"/>
-      <c r="AD15" s="81"/>
-      <c r="AE15" s="78"/>
+      <c r="AD15" s="79"/>
+      <c r="AE15" s="76"/>
       <c r="AF15" s="31"/>
       <c r="AG15" s="29"/>
       <c r="AH15" s="15"/>
       <c r="AI15" s="15"/>
       <c r="AJ15" s="23"/>
-      <c r="AK15" s="93"/>
-      <c r="AL15" s="90"/>
+      <c r="AK15" s="89"/>
+      <c r="AL15" s="86"/>
       <c r="AM15" s="3"/>
     </row>
     <row r="16" spans="1:39" s="1" customFormat="1" ht="87.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -4823,14 +5039,14 @@
       <c r="C16" s="39" t="s">
         <v>52</v>
       </c>
-      <c r="D16" s="112"/>
+      <c r="D16" s="107"/>
       <c r="E16" s="40"/>
       <c r="F16" s="13"/>
       <c r="G16" s="16"/>
       <c r="H16" s="24"/>
       <c r="I16" s="19"/>
       <c r="J16" s="24"/>
-      <c r="K16" s="70"/>
+      <c r="K16" s="68"/>
       <c r="L16" s="41"/>
       <c r="M16" s="41"/>
       <c r="N16" s="64"/>
@@ -4838,26 +5054,26 @@
       <c r="P16" s="26"/>
       <c r="Q16" s="26"/>
       <c r="R16" s="14"/>
-      <c r="S16" s="76"/>
+      <c r="S16" s="74"/>
       <c r="T16" s="41"/>
       <c r="U16" s="41"/>
       <c r="V16" s="2"/>
-      <c r="W16" s="76"/>
+      <c r="W16" s="74"/>
       <c r="X16" s="47"/>
       <c r="Y16" s="47"/>
       <c r="Z16" s="4"/>
       <c r="AA16" s="4"/>
       <c r="AB16" s="4"/>
       <c r="AC16" s="21"/>
-      <c r="AD16" s="81"/>
-      <c r="AE16" s="78"/>
+      <c r="AD16" s="79"/>
+      <c r="AE16" s="76"/>
       <c r="AF16" s="31"/>
       <c r="AG16" s="29"/>
       <c r="AH16" s="15"/>
       <c r="AI16" s="15"/>
       <c r="AJ16" s="23"/>
-      <c r="AK16" s="93"/>
-      <c r="AL16" s="90"/>
+      <c r="AK16" s="89"/>
+      <c r="AL16" s="86"/>
       <c r="AM16" s="3"/>
     </row>
     <row r="17" spans="1:39" s="1" customFormat="1" ht="87.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -4865,15 +5081,17 @@
         <v>15</v>
       </c>
       <c r="B17" s="34"/>
-      <c r="C17" s="2"/>
-      <c r="D17" s="74"/>
+      <c r="C17" s="108" t="s">
+        <v>104</v>
+      </c>
+      <c r="D17" s="72"/>
       <c r="E17" s="41"/>
       <c r="F17" s="13"/>
       <c r="G17" s="16"/>
       <c r="H17" s="24"/>
       <c r="I17" s="19"/>
       <c r="J17" s="24"/>
-      <c r="K17" s="70"/>
+      <c r="K17" s="68"/>
       <c r="L17" s="41"/>
       <c r="M17" s="41"/>
       <c r="N17" s="64"/>
@@ -4881,56 +5099,142 @@
       <c r="P17" s="26"/>
       <c r="Q17" s="26"/>
       <c r="R17" s="14"/>
-      <c r="S17" s="76"/>
+      <c r="S17" s="74"/>
       <c r="T17" s="41"/>
       <c r="U17" s="41"/>
       <c r="V17" s="2"/>
-      <c r="W17" s="76"/>
+      <c r="W17" s="74"/>
       <c r="X17" s="47"/>
       <c r="Y17" s="47"/>
       <c r="Z17" s="4"/>
       <c r="AA17" s="4"/>
       <c r="AB17" s="4"/>
       <c r="AC17" s="21"/>
-      <c r="AD17" s="81"/>
-      <c r="AE17" s="78"/>
+      <c r="AD17" s="79"/>
+      <c r="AE17" s="76"/>
       <c r="AF17" s="31"/>
       <c r="AG17" s="29"/>
       <c r="AH17" s="15"/>
       <c r="AI17" s="15"/>
       <c r="AJ17" s="23"/>
-      <c r="AK17" s="93"/>
-      <c r="AL17" s="90"/>
+      <c r="AK17" s="89"/>
+      <c r="AL17" s="86"/>
       <c r="AM17" s="3"/>
+    </row>
+    <row r="18" spans="1:39" s="1" customFormat="1" ht="87.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="109"/>
+      <c r="B18" s="110"/>
+      <c r="C18" s="111" t="s">
+        <v>105</v>
+      </c>
+      <c r="D18" s="112"/>
+      <c r="E18" s="113"/>
+      <c r="F18" s="114"/>
+      <c r="G18" s="115"/>
+      <c r="H18" s="116"/>
+      <c r="I18" s="117"/>
+      <c r="J18" s="118"/>
+      <c r="K18" s="119"/>
+      <c r="L18" s="120"/>
+      <c r="M18" s="121"/>
+      <c r="N18" s="122"/>
+      <c r="O18" s="123"/>
+      <c r="P18" s="124"/>
+      <c r="Q18" s="125"/>
+      <c r="R18" s="126"/>
+      <c r="S18" s="127"/>
+      <c r="T18" s="128"/>
+      <c r="U18" s="121"/>
+      <c r="V18" s="129"/>
+      <c r="W18" s="127"/>
+      <c r="X18" s="130"/>
+      <c r="Y18" s="131"/>
+      <c r="Z18" s="132"/>
+      <c r="AA18" s="133"/>
+      <c r="AB18" s="132"/>
+      <c r="AC18" s="134"/>
+      <c r="AD18" s="135"/>
+      <c r="AE18" s="136"/>
+      <c r="AF18" s="137"/>
+      <c r="AG18" s="138"/>
+      <c r="AH18" s="139"/>
+      <c r="AI18" s="139"/>
+      <c r="AJ18" s="139"/>
+      <c r="AK18" s="140"/>
+      <c r="AL18" s="141"/>
+      <c r="AM18" s="142"/>
+    </row>
+    <row r="19" spans="1:39" s="1" customFormat="1" ht="87.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="109"/>
+      <c r="B19" s="110"/>
+      <c r="C19" s="111" t="s">
+        <v>106</v>
+      </c>
+      <c r="D19" s="112"/>
+      <c r="E19" s="113"/>
+      <c r="F19" s="114"/>
+      <c r="G19" s="115"/>
+      <c r="H19" s="116"/>
+      <c r="I19" s="117"/>
+      <c r="J19" s="118"/>
+      <c r="K19" s="119"/>
+      <c r="L19" s="120"/>
+      <c r="M19" s="121"/>
+      <c r="N19" s="122"/>
+      <c r="O19" s="123"/>
+      <c r="P19" s="124"/>
+      <c r="Q19" s="125"/>
+      <c r="R19" s="126"/>
+      <c r="S19" s="127"/>
+      <c r="T19" s="128"/>
+      <c r="U19" s="121"/>
+      <c r="V19" s="129"/>
+      <c r="W19" s="127"/>
+      <c r="X19" s="130"/>
+      <c r="Y19" s="131"/>
+      <c r="Z19" s="132"/>
+      <c r="AA19" s="133"/>
+      <c r="AB19" s="132"/>
+      <c r="AC19" s="134"/>
+      <c r="AD19" s="135"/>
+      <c r="AE19" s="136"/>
+      <c r="AF19" s="137"/>
+      <c r="AG19" s="138"/>
+      <c r="AH19" s="139"/>
+      <c r="AI19" s="139"/>
+      <c r="AJ19" s="139"/>
+      <c r="AK19" s="140"/>
+      <c r="AL19" s="141"/>
+      <c r="AM19" s="142"/>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
-  <conditionalFormatting sqref="A3:B3 C3:E10 B4:B11 A4:A17 C12:E17 B13:B17 F3:AM17">
-    <cfRule type="endsWith" dxfId="5" priority="1" operator="endsWith" text="?">
+  <conditionalFormatting sqref="A3:B3 C3:E10 F3:AM19 B4:B11 A4:A19 C12:E19 B13:B19">
+    <cfRule type="endsWith" dxfId="4" priority="1" operator="endsWith" text="?">
       <formula>RIGHT(A3,LEN("?"))="?"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AE3:AG17">
-    <cfRule type="cellIs" dxfId="4" priority="3" operator="greaterThan">
+  <conditionalFormatting sqref="AE3:AG19">
+    <cfRule type="cellIs" dxfId="3" priority="3" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AE3:AK17">
-    <cfRule type="containsText" dxfId="3" priority="5" operator="containsText" text="0">
+  <conditionalFormatting sqref="AE3:AK19">
+    <cfRule type="containsText" dxfId="2" priority="5" operator="containsText" text="0">
       <formula>NOT(ISERROR(SEARCH("0",AE3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="2" priority="7" operator="containsText" text="J">
+    <cfRule type="containsText" dxfId="1" priority="7" operator="containsText" text="J">
       <formula>NOT(ISERROR(SEARCH("J",AE3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="1" priority="8" operator="containsText" text="N">
+    <cfRule type="containsText" dxfId="0" priority="8" operator="containsText" text="N">
       <formula>NOT(ISERROR(SEARCH("N",AE3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AH3:AK17" xr:uid="{71C80AAF-D900-484D-9411-9896D880E474}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AH3:AK19" xr:uid="{71C80AAF-D900-484D-9411-9896D880E474}">
       <formula1>"J,N"</formula1>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AE3:AG17" xr:uid="{326930F3-3C77-4222-8E18-BDC5A15AE348}">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AE3:AG19" xr:uid="{326930F3-3C77-4222-8E18-BDC5A15AE348}">
       <formula1>0</formula1>
       <formula2>10</formula2>
     </dataValidation>
@@ -4967,11 +5271,15 @@
     <hyperlink ref="C14" r:id="rId29" xr:uid="{D9345D44-2E37-4573-A18B-711CF6AA6807}"/>
     <hyperlink ref="C15" r:id="rId30" xr:uid="{151567A2-5746-463A-9F85-E3B464F76ECC}"/>
     <hyperlink ref="C16" r:id="rId31" xr:uid="{8BF53116-C1BD-44D1-A0CC-DBD9D88516E8}"/>
+    <hyperlink ref="E13" r:id="rId32" xr:uid="{EC15212B-434A-4AAD-ACE4-8055F13077B6}"/>
+    <hyperlink ref="C17" r:id="rId33" xr:uid="{CA541FF7-82B4-49E0-9174-C33E244B5D2B}"/>
+    <hyperlink ref="C18" r:id="rId34" xr:uid="{969DC642-C415-40F5-B0C7-180520D693CC}"/>
+    <hyperlink ref="C19" r:id="rId35" xr:uid="{7C2DC03F-1126-4734-A82B-88EF6376082E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId32"/>
+  <drawing r:id="rId36"/>
   <tableParts count="1">
-    <tablePart r:id="rId33"/>
+    <tablePart r:id="rId37"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>